<commit_message>
API amd statefarm test
</commit_message>
<xml_diff>
--- a/data/API.xlsx
+++ b/data/API.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneeshc\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E5CAA6-2EBA-4C0F-ADF7-F8C1886171B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21563476-4DA6-4858-A420-D64A2BCB035B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="107">
   <si>
     <t>Execution</t>
   </si>
@@ -203,101 +203,161 @@
     <t>Ocp-Apim-Subscription-Key,c5c4053a627f4e449ab85b69125e373f</t>
   </si>
   <si>
+    <t>accountId,a6b37f9f-3867-4eb9-92bd-eb3330011f3b</t>
+  </si>
+  <si>
+    <t>https://dataanywherebeta.azure-api.net/accounts-api/account</t>
+  </si>
+  <si>
+    <t>AccountsAPI_START</t>
+  </si>
+  <si>
+    <t>AccountsAPI_END</t>
+  </si>
+  <si>
+    <t>Get Accounts</t>
+  </si>
+  <si>
+    <t>https://dataanywherebeta.azure-api.net/accounts-api/accounts</t>
+  </si>
+  <si>
+    <t>[{"AccountId":"a6b37f9f-3867-4eb9-92bd-eb3330011f3b","AccountName":"Mountain's Gear's Neo BETA","PhoneNumber":"9500041445","HasChildren":false}]</t>
+  </si>
+  <si>
+    <t>LocationWriteAPI_START</t>
+  </si>
+  <si>
+    <t>LocationWriteAPI_END</t>
+  </si>
+  <si>
+    <t>Get Account with invalid Subscription</t>
+  </si>
+  <si>
+    <t>Ocp-Apim-Subscription-Key,c5c4053a627f4e449ab85b69125e373g</t>
+  </si>
+  <si>
+    <t>{ "statusCode": 401, "message": "Access denied due to invalid subscription key. Make sure to provide a valid key for an active subscription." }</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>Get Account with invalid account ID</t>
+  </si>
+  <si>
+    <t>accountId,a6b37f9f-3867-4eb9-92bd-eb3330011f3c</t>
+  </si>
+  <si>
+    <t>{"Message":"AccountID:a6b37f9f-3867-4eb9-92bd-eb3330011f3c is not bound to the current subscription."}</t>
+  </si>
+  <si>
+    <t>Get Accounts By inValid Subscription</t>
+  </si>
+  <si>
+    <t>LocationReadAPI_START</t>
+  </si>
+  <si>
+    <t>https://dataanywherebeta.azure-api.net/locations-api-read/location</t>
+  </si>
+  <si>
+    <t>Ocp-Apim-Subscription-Key,618a620ee3214799b422537a03d658b9</t>
+  </si>
+  <si>
+    <t>{"AccountID":"af70da81-0459-47a2-b3ae-9daab0c95834","LocationID":"773e82cf-e2ad-4305-9c40-01bd8c6bbd42","LocationNumber":"9000224474","ReferenceCode":"2202024","CreatedBy":"chappel.mann@gmail.com","ModifiedBy":"chappel.mann@gmail.com","Created":"2020-01-25T23:40:30.9314645Z","Modified":"2020-01-25T23:40:42.585226Z","LocationData":{"KeyFields":{"AutoDisplayPoint":"{\"Description\":null,\"DisplayMode\":null,\"Navigation\":0,\"Precision\":2,\"Type\":0,\"VerificationType\":3,\"Latitude\":24.89961,\"Longitude\":91.8751899,\"Heading\":null,\"Pitch\":null,\"Zoom\":null,\"Pin\":null}"},"DisplayPoint":{"Type":"Calculated","Latitude":24.89961,"Longitude":91.875189,"VerificationType":"DAC_Google"},"BusinessStatus":"Open","Status":"Active","BusinessName":{"Name":"The Mad Grill","LongName":"The Mad Grill","Locale":90},"PrimaryAddress":{"AddressLine1":"Manik Pir Road","AddressLine2":"Nayasarak Point","Locality":"Sylhet","PostalCode":"3100","CountryCode":"BD"},"PhoneNumbers":{"PrimaryPhoneNumber":"+8801954556677"},"MediaURLs":{"FacebookURL":"https://www.facebook.com/themadgrill/","TwitterURL":"https://www.google.com/maps?cid=9696671651361504064","LinkedInURL":"https://www.bing.com/maps?osid=05f2b478-fcec-46cf-8cec-fd03e90e9d66&amp;cp=24.900464~91.869624&amp;lvl=16&amp;imgid=28e83f0e-8669-46a5-93c8-a5957edede11&amp;v=2&amp;sV=2&amp;form=S00027","PinterestURL":"https://foursquare.com/v/mad-grill/5b8905c03149b9002c0da132","SocialNetworkURL":"https://www.tripadvisor.com/Restaurant_Review-g667997-d10825103-Reviews-The_Mad_Grill-Sylhet_City_Sylhet_Division.html"},"BusinessCategories":{"Category1":"Restaurant"}}}</t>
+  </si>
+  <si>
+    <t>LocationNumber,9000224474</t>
+  </si>
+  <si>
+    <t>Get Location</t>
+  </si>
+  <si>
+    <t>Get Location with invalid location number</t>
+  </si>
+  <si>
+    <t>{"Message":"Location with LocationNumber = 90002244745 not found for the account key specified."}</t>
+  </si>
+  <si>
+    <t>LocationNumber,90002244745</t>
+  </si>
+  <si>
+    <t>Ocp-Apim-Subscription-Key,618a620ee3214799b422537a03d658b8</t>
+  </si>
+  <si>
+    <t>LocationReadAPI_END</t>
+  </si>
+  <si>
+    <t>https://dataanywherebeta.azure-api.net/locations-api-write/location</t>
+  </si>
+  <si>
     <t>{"AccountId":"a6b37f9f-3867-4eb9-92bd-eb3330011f3b","AccountName":"Mountain's Gear's Neo BETA","PhoneNumber":"9500041445","Address":"VB 216/6 Janakpuri","City":"Delhi","Province":"DL","PostalCode":"110064","Country":"IN","CreateDate":"2020-01-15T21:04:01.913","UpdateDate":"2020-01-15T21:04:01.913","CreatorName":"mrahim@dacgroup.com","HasChildren":false,"PrimaryContactName":null,"PrimaryContactPhone":null,"PrimaryContactEmail":null,"ResellerId":"614cf1a4-cae7-4408-b6c3-c99c1c8d954f"}</t>
   </si>
   <si>
-    <t>accountId,a6b37f9f-3867-4eb9-92bd-eb3330011f3b</t>
-  </si>
-  <si>
-    <t>https://dataanywherebeta.azure-api.net/accounts-api/account</t>
-  </si>
-  <si>
-    <t>AccountsAPI_START</t>
-  </si>
-  <si>
-    <t>AccountsAPI_END</t>
-  </si>
-  <si>
-    <t>Get Accounts</t>
-  </si>
-  <si>
-    <t>https://dataanywherebeta.azure-api.net/accounts-api/accounts</t>
-  </si>
-  <si>
-    <t>[{"AccountId":"a6b37f9f-3867-4eb9-92bd-eb3330011f3b","AccountName":"Mountain's Gear's Neo BETA","PhoneNumber":"9500041445","HasChildren":false}]</t>
-  </si>
-  <si>
-    <t>LocationWriteAPI_START</t>
-  </si>
-  <si>
-    <t>LocationWriteAPI_END</t>
-  </si>
-  <si>
-    <t>Get Account with invalid Subscription</t>
-  </si>
-  <si>
-    <t>Ocp-Apim-Subscription-Key,c5c4053a627f4e449ab85b69125e373g</t>
-  </si>
-  <si>
-    <t>{ "statusCode": 401, "message": "Access denied due to invalid subscription key. Make sure to provide a valid key for an active subscription." }</t>
-  </si>
-  <si>
-    <t>401</t>
-  </si>
-  <si>
-    <t>Get Account with invalid account ID</t>
-  </si>
-  <si>
-    <t>accountId,a6b37f9f-3867-4eb9-92bd-eb3330011f3c</t>
-  </si>
-  <si>
-    <t>{"Message":"AccountID:a6b37f9f-3867-4eb9-92bd-eb3330011f3c is not bound to the current subscription."}</t>
-  </si>
-  <si>
-    <t>Get Accounts By inValid Subscription</t>
-  </si>
-  <si>
-    <t>LocationReadAPI_START</t>
-  </si>
-  <si>
-    <t>https://dataanywherebeta.azure-api.net/locations-api-read/location</t>
-  </si>
-  <si>
-    <t>Ocp-Apim-Subscription-Key,618a620ee3214799b422537a03d658b9</t>
-  </si>
-  <si>
-    <t>{"AccountID":"af70da81-0459-47a2-b3ae-9daab0c95834","LocationID":"773e82cf-e2ad-4305-9c40-01bd8c6bbd42","LocationNumber":"9000224474","ReferenceCode":"2202024","CreatedBy":"chappel.mann@gmail.com","ModifiedBy":"chappel.mann@gmail.com","Created":"2020-01-25T23:40:30.9314645Z","Modified":"2020-01-25T23:40:42.585226Z","LocationData":{"KeyFields":{"AutoDisplayPoint":"{\"Description\":null,\"DisplayMode\":null,\"Navigation\":0,\"Precision\":2,\"Type\":0,\"VerificationType\":3,\"Latitude\":24.89961,\"Longitude\":91.8751899,\"Heading\":null,\"Pitch\":null,\"Zoom\":null,\"Pin\":null}"},"DisplayPoint":{"Type":"Calculated","Latitude":24.89961,"Longitude":91.875189,"VerificationType":"DAC_Google"},"BusinessStatus":"Open","Status":"Active","BusinessName":{"Name":"The Mad Grill","LongName":"The Mad Grill","Locale":90},"PrimaryAddress":{"AddressLine1":"Manik Pir Road","AddressLine2":"Nayasarak Point","Locality":"Sylhet","PostalCode":"3100","CountryCode":"BD"},"PhoneNumbers":{"PrimaryPhoneNumber":"+8801954556677"},"MediaURLs":{"FacebookURL":"https://www.facebook.com/themadgrill/","TwitterURL":"https://www.google.com/maps?cid=9696671651361504064","LinkedInURL":"https://www.bing.com/maps?osid=05f2b478-fcec-46cf-8cec-fd03e90e9d66&amp;cp=24.900464~91.869624&amp;lvl=16&amp;imgid=28e83f0e-8669-46a5-93c8-a5957edede11&amp;v=2&amp;sV=2&amp;form=S00027","PinterestURL":"https://foursquare.com/v/mad-grill/5b8905c03149b9002c0da132","SocialNetworkURL":"https://www.tripadvisor.com/Restaurant_Review-g667997-d10825103-Reviews-The_Mad_Grill-Sylhet_City_Sylhet_Division.html"},"BusinessCategories":{"Category1":"Restaurant"}}}</t>
-  </si>
-  <si>
-    <t>LocationNumber,9000224474</t>
-  </si>
-  <si>
-    <t>Get Location</t>
-  </si>
-  <si>
-    <t>Get Location with invalid location number</t>
-  </si>
-  <si>
-    <t>{"Message":"Location with LocationNumber = 90002244745 not found for the account key specified."}</t>
-  </si>
-  <si>
-    <t>LocationNumber,90002244745</t>
-  </si>
-  <si>
-    <t>Ocp-Apim-Subscription-Key,618a620ee3214799b422537a03d658b8</t>
-  </si>
-  <si>
-    <t>LocationReadAPI_END</t>
-  </si>
-  <si>
-    <t>https://dataanywherebeta.azure-api.net/locations-api-write/location</t>
+    <t>LocationID,05f6fee4-553d-414c-bd80-4f82a3f7fc41</t>
+  </si>
+  <si>
+    <t>LocationID,05f6fee4-553d-414c-bd80-4f82a3f7fc42</t>
+  </si>
+  <si>
+    <t>{"AccountID":"a6b37f9f-3867-4eb9-92bd-eb3330011f3b","LocationID":"05f6fee4-553d-414c-bd80-4f82a3f7fc41","LocationNumber":"9000224268","CreatedBy":"dac_ra_beta1@dacgroup.com","ModifiedBy":"dac_ra_beta1@dacgroup.com","Created":"2020-01-15T21:13:08.9808306Z","Modified":"2020-01-15T21:13:26.8742665Z","LocationData":{"KeyFields":{"AutoDisplayPoint":"{\"Description\":null,\"DisplayMode\":null,\"Navigation\":0,\"Precision\":3,\"Type\":0,\"VerificationType\":3,\"Latitude\":50.4853437,\"Longitude\":-104.6174239,\"Heading\":null,\"Pitch\":null,\"Zoom\":null,\"Pin\":null}"},"DisplayPoint":{"Type":"Calculated","Latitude":50.485343,"Longitude":-104.617423,"VerificationType":"DAC_Google"},"BusinessStatus":"Open","Status":"Active","BusinessName":{"Name":"Mountain Gear","LongName":"Mountain Gear B","Locale":48},"PrimaryAddress":{"AddressLine1":"1180 W State St","Locality":"Regina","Region":"SK","PostalCode":"S4R 8E2","CountryCode":"CA"},"PhoneNumbers":{"PrimaryPhoneNumber":"+13065430236"},"MediaURLs":{},"BusinessCategories":{"Category1":"Outdoor Sports Store"},"PhotoURLs":[]}}</t>
+  </si>
+  <si>
+    <t>Get Location with invalid location ID</t>
+  </si>
+  <si>
+    <t>Get Account with invalid Subscription and Account ID</t>
+  </si>
+  <si>
+    <t>GetAccountByAccountID</t>
+  </si>
+  <si>
+    <t>Get Location with invalid location number and inValid Subscription</t>
+  </si>
+  <si>
+    <t>Get Location By inValid Subscription &amp; location ID</t>
+  </si>
+  <si>
+    <t>Get Locations</t>
+  </si>
+  <si>
+    <t>Get Locations By inValid Subscription</t>
+  </si>
+  <si>
+    <t>Get Locations with invalid account ID</t>
+  </si>
+  <si>
+    <t>Get Locations By inValid Subscription &amp; account id ID</t>
+  </si>
+  <si>
+    <t>https://dataanywherebeta.azure-api.net/locations-api-write/locations</t>
+  </si>
+  <si>
+    <t>AccountID,a6b37f9f-3867-4eb9-92bd-eb3330011f3b</t>
+  </si>
+  <si>
+    <t>AccountID,a6b37f9f-3867-4eb9-92bd-eb3330011f3c</t>
+  </si>
+  <si>
+    <t>{"ContinuationToken":"%5b%7b%22token%22%3a%22%2bRID%3a%7efxp-AKdCbvNLsQIAAAAACA%3d%3d%23RT%3a1%23TRC%3a25%23ISV%3a2%23IEO%3a65551%23FPC%3aAggKAAAAACAAAAoAAAAAIAAACgAAAAAgAAAoAEIxAPgDABqAYQAAA5mBMYADgEeADoBFgQHAAGCbgXEAAGA2gDEFAMA%3d%22%2c%22range%22%3a%7b%22min%22%3a%22%22%2c%22max%22%3a%2205C1E1EDCF6FCA%22%7d%7d%5d","Count":25,"Data":[{"LocationID":"3a000feb-cc28-439e-86fd-a00cedbb5288","LocationNumber":"9000224316","ReferenceCode":"9003017","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+17054884444","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"85 Dunlop St W","Locality":"Barrie","Region":"ON","PostalCode":"L4N 1A5","CountryCode":"CA"}},{"LocationID":"24dffa05-4d3c-40c9-930e-2116ad20a36f","LocationNumber":"9000224314","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+17054884444","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"85 Dunlop St W","Locality":"Barrie","Region":"ON","PostalCode":"L4N 1A5","CountryCode":"CA"}},{"LocationID":"0a2cc9c6-a838-4668-885b-53ce1fd8b7e0","LocationNumber":"9000224312","ReferenceCode":"9003014","LongBusinessName":"Mountain Gear A","PrimaryPhoneNumber":"+14076366493","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1950 6th Ave","Locality":"Seattle","Region":"WA","PostalCode":"98101","CountryCode":"US"}},{"LocationID":"d2696bc5-5a8b-4e41-be76-96a91818ebcf","LocationNumber":"9000224309","ReferenceCode":"9002995","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+14356353188","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1180 W State St","Locality":"Hurricane","Region":"UT","PostalCode":"84737","CountryCode":"US"}},{"LocationID":"2e174a11-aeab-463f-8872-70b249f858bb","LocationNumber":"9000224310","ReferenceCode":"Inceptos","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+13064457475","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"11102 Railway Ave E","Locality":"North Battleford","Region":"SK","PostalCode":"S9A 2X6","CountryCode":"CA"}},{"LocationID":"d2df7f02-ae69-406d-a8dd-5b30d27b997a","LocationNumber":"9000224307","ReferenceCode":"9003003","LongBusinessName":"Mountain Gear A","PrimaryPhoneNumber":"+12063749596","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1950 6th Ave","Locality":"Seattle","Region":"WA","PostalCode":"98101","CountryCode":"US"}},{"LocationID":"e3533dc1-4f61-460a-9697-0a7648f43e94","LocationNumber":"9000224306","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+13069334262","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"115 Marquis Dr W","Locality":"Saskatoon","Region":"SK","PostalCode":"S7R 1C7","CountryCode":"CA"}},{"LocationID":"d142a839-a904-423d-a0b4-369642ad7600","LocationNumber":"9000224302","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+14356353188","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1180 W State St","Locality":"Hurricane","Region":"UT","PostalCode":"84737","CountryCode":"US"}},{"LocationID":"b39f824b-5575-4c54-9c56-20fb93c47c0b","LocationNumber":"9000224301","ReferenceCode":"9003026","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+12063749596","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1950 6th Ave","Locality":"Seattle","Region":"WA","PostalCode":"98101","CountryCode":"US"}},{"LocationID":"164c0a1f-3f7e-4eef-b44f-be55711a801f","LocationNumber":"9000224297","ReferenceCode":"9003027","LongBusinessName":"Egestas","PrimaryPhoneNumber":"+14068834125","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"111 Fulton St","Locality":"New York","Region":"NY","PostalCode":"10038","CountryCode":"US"}},{"LocationID":"35a434be-ccd6-489f-bb31-f2e4d4dd99ac","LocationNumber":"9000224294","ReferenceCode":"9003015","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+12063749596","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1950 6th Ave","Locality":"Seattle","Region":"WA","PostalCode":"98101","CountryCode":"US"}},{"LocationID":"25d447bf-fcb9-416b-969b-0b4abc5cb40e","LocationNumber":"9000224290","ReferenceCode":"9003011","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+13064457475","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"11102 Railway Ave E","Locality":"North Battleford","Region":"SK","PostalCode":"S9A 2X6","CountryCode":"CA"}},{"LocationID":"e6f6ded5-0f60-4ca3-bbba-adbb0b202aef","LocationNumber":"9000224291","ReferenceCode":"9003009","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+12703885347","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"82 US-62","Locality":"Eddyville","Region":"KY","PostalCode":"42038","CountryCode":"US"}},{"LocationID":"ec91f10c-e5f1-4dc3-9afa-b2e1a5a9e1c4","LocationNumber":"9000224288","ReferenceCode":"9003021","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+12703885347","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"111 W 40th St","Locality":"New York","Region":"NY","PostalCode":"10018","CountryCode":"US"}},{"LocationID":"0defac7f-aa9d-4b3e-b6a1-b3fc30819ee8","LocationNumber":"9000224284","ReferenceCode":"0702pl","LongBusinessName":"Norauto GDAŃSK","PrimaryPhoneNumber":"+48587694700","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"c.h. auchan","AddressLine2":"ul. szczęśliwa 9","Locality":"gdańsk","PostalCode":"80-176","CountryCode":"PL"}},{"LocationID":"beff059c-38d7-46b0-a9ab-de51cb5068ff","LocationNumber":"9000224281","ReferenceCode":"ID_Ref","LongBusinessName":"Indonesia","PrimaryPhoneNumber":"+626274124921","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"Mediterranea Restaurant by Kamil","AddressLine2":"Mantrijeron","AddressLine3":"Tirtodipuran","Locality":"Yogyakarta City","Region":"YO","PostalCode":"55143","CountryCode":"ID"}},{"LocationID":"ba0fab29-dc33-4020-966e-828d7e903f4e","LocationNumber":"9000224280","ReferenceCode":"9003006","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+14356353188","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1180 W State St","Locality":"Hurricane","Region":"UT","PostalCode":"84737","CountryCode":"US"}},{"LocationID":"1af11eee-60f0-4819-937f-e0af65529a4c","LocationNumber":"9000224277","ReferenceCode":"9003028","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+17054884444","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"85 Dunlop St W","Locality":"Barrie","Region":"ON","PostalCode":"L4N 1A5","CountryCode":"CA"}},{"LocationID":"266f44fb-da1e-4ec8-98eb-28356dd62ab1","LocationNumber":"9000224278","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+17054884444","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"85 Dunlop St W","Locality":"Barrie","Region":"ON","PostalCode":"L4N 1A5","CountryCode":"CA"}},{"LocationID":"bf123446-fa6a-41dc-975e-a24d840d8096","LocationNumber":"9000224272","ReferenceCode":"9003005","LongBusinessName":"Imperdiet","PrimaryPhoneNumber":"+17054884444","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"85 Dunlop St W","Locality":"Barrie","Region":"ON","PostalCode":"L4N 1A5","CountryCode":"CA"}},{"LocationID":"05f6fee4-553d-414c-bd80-4f82a3f7fc41","LocationNumber":"9000224268","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+13065430236","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1180 W State St","Locality":"Regina","Region":"SK","PostalCode":"S4R 8E2","CountryCode":"CA"}},{"LocationID":"a70b1727-afb0-4fee-a57e-556e679cacdc","LocationNumber":"9000224267","ReferenceCode":"9003002","LongBusinessName":"Ultrices","PrimaryPhoneNumber":"+13069334262","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"115 Marquis Dr W","Locality":"Saskatoon","Region":"SK","PostalCode":"S7R 1C7","CountryCode":"CA"}},{"LocationID":"e5bd8e8d-c870-4a46-b04d-4d5baab3eb34","LocationNumber":"9000224263","LongBusinessName":"Mountain Gear B","PrimaryPhoneNumber":"+12503741718","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1751 Trans-Canada Hwy","Locality":"Kamloops","Region":"BC","PostalCode":"V2C 3Z6","CountryCode":"CA"}},{"LocationID":"3107799d-7aca-43f3-a03f-6e066e78bd83","LocationNumber":"9000224262","LongBusinessName":"Mountain Gear C","PrimaryPhoneNumber":"+13069558669","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1608 8 St E","Locality":"Saskatoon","Region":"SK","PostalCode":"S7H 0T3","CountryCode":"CA"}},{"LocationID":"a751d7c4-06b5-47e2-979f-c36efbc5aa38","LocationNumber":"9000224261","ReferenceCode":"9003012","LongBusinessName":"Pellentesque","PrimaryPhoneNumber":"+12503741718","BusinessStatus":"Open","Status":"Active","PrimaryAddress":{"AddressLine1":"1751 Trans-Canada Hwy","Locality":"Kamloops","Region":"BC","PostalCode":"V2C 3Z6","CountryCode":"CA"}}]}</t>
+  </si>
+  <si>
+    <t>https://dataanywhere-api-beta.azurewebsites.net/api/internal/usage</t>
+  </si>
+  <si>
+    <t>Get Usage(Internal)</t>
+  </si>
+  <si>
+    <t>Ocp-Apim-Subscription-Key,22C71F28A3D149B49E4A22B6F043B6CF</t>
+  </si>
+  <si>
+    <t>DA_Subscription_START</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +410,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF585858"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -384,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -412,8 +484,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -886,25 +960,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C34382D-1C7F-4057-B1C8-D7F3111724BD}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
-    <col min="3" max="3" width="74.42578125" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
+    <col min="3" max="3" width="69" customWidth="1"/>
     <col min="4" max="4" width="61.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" customWidth="1"/>
+    <col min="7" max="7" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -939,24 +1013,26 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="B3" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>1</v>
@@ -964,22 +1040,22 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>1</v>
@@ -988,43 +1064,45 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>72</v>
+      <c r="E5" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>64</v>
+        <v>91</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>1</v>
@@ -1032,107 +1110,105 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="E15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>1</v>
@@ -1140,160 +1216,434 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="18" t="s">
+      <c r="C17" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="C26" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H14:H16 H3:H7 H22:H24" xr:uid="{6C167517-751F-455B-A196-89F837878FC8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8 H15:H18 H24:H31 H37:H40" xr:uid="{6C167517-751F-455B-A196-89F837878FC8}">
       <formula1>"RUN,NO-RUN"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" xr:uid="{83C83BCB-B139-4A51-8B0B-D275991D9510}"/>
+    <hyperlink ref="C39" r:id="rId1" xr:uid="{64AC546F-EE73-4966-A05F-FDE15061469F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>